<commit_message>
Data Feed File Updated
</commit_message>
<xml_diff>
--- a/Data_Feed_File.xlsx
+++ b/Data_Feed_File.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGABRANI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imranjuma/Desktop/covasim-1.7.6/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EC0C78-B3C2-CB4E-895B-C9C09CCE0259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9645" yWindow="465" windowWidth="15960" windowHeight="13575"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -38,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -398,19 +407,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="A262" sqref="A262"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="A335" sqref="A335:XFD335"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -421,21 +430,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>43852</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>43853</v>
       </c>
@@ -446,7 +455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>43854</v>
       </c>
@@ -457,7 +466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>43855</v>
       </c>
@@ -468,7 +477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>43856</v>
       </c>
@@ -479,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>43857</v>
       </c>
@@ -490,7 +499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>43858</v>
       </c>
@@ -501,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>43859</v>
       </c>
@@ -512,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>43860</v>
       </c>
@@ -523,7 +532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>43861</v>
       </c>
@@ -534,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>43862</v>
       </c>
@@ -545,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>43863</v>
       </c>
@@ -556,7 +565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>43864</v>
       </c>
@@ -567,7 +576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>43865</v>
       </c>
@@ -578,7 +587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>43866</v>
       </c>
@@ -589,7 +598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>43867</v>
       </c>
@@ -600,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>43868</v>
       </c>
@@ -611,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>43869</v>
       </c>
@@ -622,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>43870</v>
       </c>
@@ -633,7 +642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>43871</v>
       </c>
@@ -644,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>43872</v>
       </c>
@@ -655,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>43873</v>
       </c>
@@ -666,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>43874</v>
       </c>
@@ -677,7 +686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>43875</v>
       </c>
@@ -688,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>43876</v>
       </c>
@@ -699,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>43877</v>
       </c>
@@ -710,7 +719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>43878</v>
       </c>
@@ -721,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>43879</v>
       </c>
@@ -732,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>43880</v>
       </c>
@@ -743,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>43881</v>
       </c>
@@ -754,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>43882</v>
       </c>
@@ -765,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>43883</v>
       </c>
@@ -776,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>43884</v>
       </c>
@@ -787,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>43885</v>
       </c>
@@ -798,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>43886</v>
       </c>
@@ -809,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>43887</v>
       </c>
@@ -820,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>43888</v>
       </c>
@@ -831,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>43889</v>
       </c>
@@ -842,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>43890</v>
       </c>
@@ -853,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>43891</v>
       </c>
@@ -864,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>43892</v>
       </c>
@@ -875,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43893</v>
       </c>
@@ -886,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>43894</v>
       </c>
@@ -897,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>43895</v>
       </c>
@@ -908,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>43896</v>
       </c>
@@ -919,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>43897</v>
       </c>
@@ -930,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>43898</v>
       </c>
@@ -941,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>43899</v>
       </c>
@@ -952,7 +961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>43900</v>
       </c>
@@ -963,7 +972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>43901</v>
       </c>
@@ -974,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>43902</v>
       </c>
@@ -985,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>43903</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>43904</v>
       </c>
@@ -1007,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>43905</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>43906</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>43907</v>
       </c>
@@ -1040,7 +1049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>43908</v>
       </c>
@@ -1051,7 +1060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>43909</v>
       </c>
@@ -1062,7 +1071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>43910</v>
       </c>
@@ -1073,7 +1082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>43911</v>
       </c>
@@ -1084,7 +1093,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>43912</v>
       </c>
@@ -1095,7 +1104,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>43913</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>43914</v>
       </c>
@@ -1117,7 +1126,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>43915</v>
       </c>
@@ -1128,7 +1137,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>43916</v>
       </c>
@@ -1139,7 +1148,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>43917</v>
       </c>
@@ -1150,7 +1159,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>43918</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>43919</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>43920</v>
       </c>
@@ -1183,7 +1192,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>43921</v>
       </c>
@@ -1194,7 +1203,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>43922</v>
       </c>
@@ -1205,7 +1214,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>43923</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>43924</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>43925</v>
       </c>
@@ -1238,7 +1247,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>43926</v>
       </c>
@@ -1249,7 +1258,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>43927</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>43928</v>
       </c>
@@ -1271,7 +1280,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>43929</v>
       </c>
@@ -1282,7 +1291,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>43930</v>
       </c>
@@ -1293,7 +1302,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>43931</v>
       </c>
@@ -1304,7 +1313,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>43932</v>
       </c>
@@ -1315,7 +1324,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>43933</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>43934</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>43935</v>
       </c>
@@ -1348,7 +1357,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>43936</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>43937</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>43938</v>
       </c>
@@ -1381,7 +1390,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>43939</v>
       </c>
@@ -1392,7 +1401,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>43940</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>43941</v>
       </c>
@@ -1414,7 +1423,7 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>43942</v>
       </c>
@@ -1425,7 +1434,7 @@
         <v>1910</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>43943</v>
       </c>
@@ -1436,7 +1445,7 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>43944</v>
       </c>
@@ -1447,7 +1456,7 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>43945</v>
       </c>
@@ -1458,7 +1467,7 @@
         <v>2402</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>43946</v>
       </c>
@@ -1469,7 +1478,7 @@
         <v>2571</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>43947</v>
       </c>
@@ -1480,7 +1489,7 @@
         <v>2687</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>43948</v>
       </c>
@@ -1491,7 +1500,7 @@
         <v>2841</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>43949</v>
       </c>
@@ -1502,7 +1511,7 @@
         <v>2983</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>43950</v>
       </c>
@@ -1513,7 +1522,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>43951</v>
       </c>
@@ -1524,7 +1533,7 @@
         <v>3310</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>43952</v>
       </c>
@@ -1535,7 +1544,7 @@
         <v>3537</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>43953</v>
       </c>
@@ -1546,7 +1555,7 @@
         <v>3684</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>43954</v>
       </c>
@@ -1557,7 +1566,7 @@
         <v>3795</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>43955</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>4003</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>43956</v>
       </c>
@@ -1579,7 +1588,7 @@
         <v>4190</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>43957</v>
       </c>
@@ -1590,7 +1599,7 @@
         <v>4366</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>43958</v>
       </c>
@@ -1601,7 +1610,7 @@
         <v>4541</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>43959</v>
       </c>
@@ -1612,7 +1621,7 @@
         <v>4697</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>43960</v>
       </c>
@@ -1623,7 +1632,7 @@
         <v>4823</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>43961</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>4991</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>43962</v>
       </c>
@@ -1645,7 +1654,7 @@
         <v>5115</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>43963</v>
       </c>
@@ -1656,7 +1665,7 @@
         <v>5300</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>43964</v>
       </c>
@@ -1667,7 +1676,7 @@
         <v>5425</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>43965</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>5592</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>43966</v>
       </c>
@@ -1689,7 +1698,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>43967</v>
       </c>
@@ -1700,7 +1709,7 @@
         <v>5800</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>43968</v>
       </c>
@@ -1711,7 +1720,7 @@
         <v>5903</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>43969</v>
       </c>
@@ -1722,7 +1731,7 @@
         <v>5960</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>43970</v>
       </c>
@@ -1733,7 +1742,7 @@
         <v>6028</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>43971</v>
       </c>
@@ -1744,7 +1753,7 @@
         <v>6150</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>43972</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>6267</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>43973</v>
       </c>
@@ -1766,7 +1775,7 @@
         <v>6360</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>43974</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>6466</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>43975</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>6534</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>43976</v>
       </c>
@@ -1799,7 +1808,7 @@
         <v>6655</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>43977</v>
       </c>
@@ -1810,7 +1819,7 @@
         <v>6753</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>43978</v>
       </c>
@@ -1821,7 +1830,7 @@
         <v>6876</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>43979</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>6982</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>43980</v>
       </c>
@@ -1843,7 +1852,7 @@
         <v>7063</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>43981</v>
       </c>
@@ -1854,7 +1863,7 @@
         <v>7159</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>43982</v>
       </c>
@@ -1865,7 +1874,7 @@
         <v>7374</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>43983</v>
       </c>
@@ -1876,7 +1885,7 @@
         <v>7404</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>43984</v>
       </c>
@@ -1887,7 +1896,7 @@
         <v>7478</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>43985</v>
       </c>
@@ -1898,7 +1907,7 @@
         <v>7579</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>43986</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v>7717</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>43987</v>
       </c>
@@ -1920,7 +1929,7 @@
         <v>7778</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>43988</v>
       </c>
@@ -1931,7 +1940,7 @@
         <v>7850</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>43989</v>
       </c>
@@ -1942,7 +1951,7 @@
         <v>7877</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>43990</v>
       </c>
@@ -1953,7 +1962,7 @@
         <v>7910</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>43991</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>7970</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>43992</v>
       </c>
@@ -1975,7 +1984,7 @@
         <v>8038</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>43993</v>
       </c>
@@ -1986,7 +1995,7 @@
         <v>8071</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>43994</v>
       </c>
@@ -1997,7 +2006,7 @@
         <v>8125</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>43995</v>
       </c>
@@ -2008,7 +2017,7 @@
         <v>8183</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>43996</v>
       </c>
@@ -2019,7 +2028,7 @@
         <v>8218</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>43997</v>
       </c>
@@ -2030,7 +2039,7 @@
         <v>8228</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>43998</v>
       </c>
@@ -2041,7 +2050,7 @@
         <v>8271</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>43999</v>
       </c>
@@ -2052,7 +2061,7 @@
         <v>8312</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>44000</v>
       </c>
@@ -2063,7 +2072,7 @@
         <v>8361</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>44001</v>
       </c>
@@ -2074,7 +2083,7 @@
         <v>8408</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>44002</v>
       </c>
@@ -2085,7 +2094,7 @@
         <v>8466</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>44003</v>
       </c>
@@ -2096,7 +2105,7 @@
         <v>8482</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>44004</v>
       </c>
@@ -2107,7 +2116,7 @@
         <v>8494</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>44005</v>
       </c>
@@ -2118,7 +2127,7 @@
         <v>8512</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>44006</v>
       </c>
@@ -2129,7 +2138,7 @@
         <v>8544</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>44007</v>
       </c>
@@ -2140,7 +2149,7 @@
         <v>8567</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>44008</v>
       </c>
@@ -2151,7 +2160,7 @@
         <v>8571</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>44009</v>
       </c>
@@ -2162,7 +2171,7 @@
         <v>8576</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>44010</v>
       </c>
@@ -2173,7 +2182,7 @@
         <v>8582</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>44011</v>
       </c>
@@ -2184,7 +2193,7 @@
         <v>8628</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>44012</v>
       </c>
@@ -2195,7 +2204,7 @@
         <v>8650</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>44013</v>
       </c>
@@ -2206,7 +2215,7 @@
         <v>8678</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>44014</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>44015</v>
       </c>
@@ -2228,7 +2237,7 @@
         <v>8722</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>44016</v>
       </c>
@@ -2239,7 +2248,7 @@
         <v>8732</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>44017</v>
       </c>
@@ -2250,7 +2259,7 @@
         <v>8739</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>44018</v>
       </c>
@@ -2261,7 +2270,7 @@
         <v>8748</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>44019</v>
       </c>
@@ -2272,7 +2281,7 @@
         <v>8765</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>44020</v>
       </c>
@@ -2283,7 +2292,7 @@
         <v>8786</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>44021</v>
       </c>
@@ -2294,7 +2303,7 @@
         <v>8797</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>44022</v>
       </c>
@@ -2305,7 +2314,7 @@
         <v>8811</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>44023</v>
       </c>
@@ -2316,7 +2325,7 @@
         <v>8818</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>44024</v>
       </c>
@@ -2327,7 +2336,7 @@
         <v>8829</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>44025</v>
       </c>
@@ -2338,7 +2347,7 @@
         <v>8836</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>44026</v>
       </c>
@@ -2349,7 +2358,7 @@
         <v>8845</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>44027</v>
       </c>
@@ -2360,7 +2369,7 @@
         <v>8857</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>44028</v>
       </c>
@@ -2371,7 +2380,7 @@
         <v>8875</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>44029</v>
       </c>
@@ -2382,7 +2391,7 @@
         <v>8884</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>44030</v>
       </c>
@@ -2393,7 +2402,7 @@
         <v>8892</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>44031</v>
       </c>
@@ -2404,7 +2413,7 @@
         <v>8896</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>44032</v>
       </c>
@@ -2415,7 +2424,7 @@
         <v>8902</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>44033</v>
       </c>
@@ -2426,7 +2435,7 @@
         <v>8908</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>44034</v>
       </c>
@@ -2437,7 +2446,7 @@
         <v>8913</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>44035</v>
       </c>
@@ -2448,7 +2457,7 @@
         <v>8919</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>44036</v>
       </c>
@@ -2459,7 +2468,7 @@
         <v>8923</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>44037</v>
       </c>
@@ -2470,7 +2479,7 @@
         <v>8929</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>44038</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>8934</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>44039</v>
       </c>
@@ -2492,7 +2501,7 @@
         <v>8945</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>44040</v>
       </c>
@@ -2503,7 +2512,7 @@
         <v>8957</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>44041</v>
       </c>
@@ -2514,7 +2523,7 @@
         <v>8962</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>44042</v>
       </c>
@@ -2525,7 +2534,7 @@
         <v>8974</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>44043</v>
       </c>
@@ -2536,7 +2545,7 @@
         <v>8980</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>44044</v>
       </c>
@@ -2547,7 +2556,7 @@
         <v>8986</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>44045</v>
       </c>
@@ -2559,7 +2568,7 @@
       </c>
       <c r="E196" s="5"/>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>44046</v>
       </c>
@@ -2571,7 +2580,7 @@
       </c>
       <c r="E197" s="5"/>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>44047</v>
       </c>
@@ -2583,7 +2592,7 @@
       </c>
       <c r="E198" s="5"/>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>44048</v>
       </c>
@@ -2595,7 +2604,7 @@
       </c>
       <c r="E199" s="5"/>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>44049</v>
       </c>
@@ -2607,7 +2616,7 @@
       </c>
       <c r="E200" s="5"/>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>44050</v>
       </c>
@@ -2619,7 +2628,7 @@
       </c>
       <c r="E201" s="5"/>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>44051</v>
       </c>
@@ -2631,7 +2640,7 @@
       </c>
       <c r="E202" s="5"/>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>44052</v>
       </c>
@@ -2643,7 +2652,7 @@
       </c>
       <c r="E203" s="5"/>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>44053</v>
       </c>
@@ -2655,7 +2664,7 @@
       </c>
       <c r="E204" s="5"/>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>44054</v>
       </c>
@@ -2667,7 +2676,7 @@
       </c>
       <c r="E205" s="5"/>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>44055</v>
       </c>
@@ -2679,7 +2688,7 @@
       </c>
       <c r="E206" s="5"/>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>44056</v>
       </c>
@@ -2691,7 +2700,7 @@
       </c>
       <c r="E207" s="5"/>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>44057</v>
       </c>
@@ -2703,7 +2712,7 @@
       </c>
       <c r="E208" s="5"/>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>44058</v>
       </c>
@@ -2715,7 +2724,7 @@
       </c>
       <c r="E209" s="5"/>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>44059</v>
       </c>
@@ -2727,7 +2736,7 @@
       </c>
       <c r="E210" s="5"/>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>44060</v>
       </c>
@@ -2739,7 +2748,7 @@
       </c>
       <c r="E211" s="5"/>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>44061</v>
       </c>
@@ -2751,7 +2760,7 @@
       </c>
       <c r="E212" s="5"/>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>44062</v>
       </c>
@@ -2763,7 +2772,7 @@
       </c>
       <c r="E213" s="5"/>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>44063</v>
       </c>
@@ -2775,7 +2784,7 @@
       </c>
       <c r="E214" s="5"/>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>44064</v>
       </c>
@@ -2787,7 +2796,7 @@
       </c>
       <c r="E215" s="5"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>44065</v>
       </c>
@@ -2799,7 +2808,7 @@
       </c>
       <c r="E216" s="5"/>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>44066</v>
       </c>
@@ -2811,7 +2820,7 @@
       </c>
       <c r="E217" s="5"/>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>44067</v>
       </c>
@@ -2823,7 +2832,7 @@
       </c>
       <c r="E218" s="5"/>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>44068</v>
       </c>
@@ -2835,7 +2844,7 @@
       </c>
       <c r="E219" s="5"/>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>44069</v>
       </c>
@@ -2847,7 +2856,7 @@
       </c>
       <c r="E220" s="5"/>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>44070</v>
       </c>
@@ -2859,7 +2868,7 @@
       </c>
       <c r="E221" s="5"/>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>44071</v>
       </c>
@@ -2871,7 +2880,7 @@
       </c>
       <c r="E222" s="5"/>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>44072</v>
       </c>
@@ -2882,7 +2891,7 @@
         <v>9161</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>44073</v>
       </c>
@@ -2893,7 +2902,7 @@
         <v>9164</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>44074</v>
       </c>
@@ -2904,7 +2913,7 @@
         <v>9173</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>44075</v>
       </c>
@@ -2915,7 +2924,7 @@
         <v>9179</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>44076</v>
       </c>
@@ -2926,7 +2935,7 @@
         <v>9182</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>44077</v>
       </c>
@@ -2937,7 +2946,7 @@
         <v>9189</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>44078</v>
       </c>
@@ -2948,7 +2957,7 @@
         <v>9190</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>44079</v>
       </c>
@@ -2959,7 +2968,7 @@
         <v>9192</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>44080</v>
       </c>
@@ -2970,7 +2979,7 @@
         <v>9194</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>44081</v>
       </c>
@@ -2981,7 +2990,7 @@
         <v>9196</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>44082</v>
       </c>
@@ -2992,7 +3001,7 @@
         <v>9203</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>44083</v>
       </c>
@@ -3003,7 +3012,7 @@
         <v>9204</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>44084</v>
       </c>
@@ -3014,7 +3023,7 @@
         <v>9213</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>44085</v>
       </c>
@@ -3025,7 +3034,7 @@
         <v>9214</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>44086</v>
       </c>
@@ -3036,7 +3045,7 @@
         <v>9220</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>44087</v>
       </c>
@@ -3047,7 +3056,7 @@
         <v>9220</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>44088</v>
       </c>
@@ -3058,7 +3067,7 @@
         <v>9229</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>44089</v>
       </c>
@@ -3069,7 +3078,7 @@
         <v>9239</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>44090</v>
       </c>
@@ -3080,7 +3089,7 @@
         <v>9244</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>44091</v>
       </c>
@@ -3091,7 +3100,7 @@
         <v>9249</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>44092</v>
       </c>
@@ -3102,7 +3111,7 @@
         <v>9256</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>44093</v>
       </c>
@@ -3113,7 +3122,7 @@
         <v>9262</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>44094</v>
       </c>
@@ -3124,7 +3133,7 @@
         <v>9267</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>44095</v>
       </c>
@@ -3135,7 +3144,7 @@
         <v>9279</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>44096</v>
       </c>
@@ -3146,7 +3155,7 @@
         <v>9286</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>44097</v>
       </c>
@@ -3157,7 +3166,7 @@
         <v>9294</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>44098</v>
       </c>
@@ -3168,7 +3177,7 @@
         <v>9297</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>44099</v>
       </c>
@@ -3179,7 +3188,7 @@
         <v>9306</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>44100</v>
       </c>
@@ -3190,7 +3199,7 @@
         <v>9313</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>44101</v>
       </c>
@@ -3201,7 +3210,7 @@
         <v>9318</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>44102</v>
       </c>
@@ -3212,7 +3221,7 @@
         <v>9328</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>44103</v>
       </c>
@@ -3223,7 +3232,7 @@
         <v>9340</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>44104</v>
       </c>
@@ -3234,7 +3243,7 @@
         <v>9346</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>44105</v>
       </c>
@@ -3245,7 +3254,7 @@
         <v>9368</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>44106</v>
       </c>
@@ -3256,7 +3265,7 @@
         <v>9466</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>44107</v>
       </c>
@@ -3267,7 +3276,7 @@
         <v>9488</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>44108</v>
       </c>
@@ -3278,7 +3287,7 @@
         <v>9533</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>44109</v>
       </c>
@@ -3289,7 +3298,7 @@
         <v>9560</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>44110</v>
       </c>
@@ -3300,10 +3309,788 @@
         <v>9582</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" s="1"/>
-    </row>
-    <row r="1048576" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B262">
+        <v>175380</v>
+      </c>
+      <c r="C262">
+        <v>9593</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B263">
+        <v>177730</v>
+      </c>
+      <c r="C263">
+        <v>9609</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B264">
+        <v>180625</v>
+      </c>
+      <c r="C264">
+        <v>9638</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B265">
+        <v>182767</v>
+      </c>
+      <c r="C265">
+        <v>9661</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B266">
+        <v>184403</v>
+      </c>
+      <c r="C266">
+        <v>9666</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B267">
+        <v>185378</v>
+      </c>
+      <c r="C267">
+        <v>9680</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B268">
+        <v>189489</v>
+      </c>
+      <c r="C268">
+        <v>9707</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" s="1">
+        <v>44118</v>
+      </c>
+      <c r="B269">
+        <v>192064</v>
+      </c>
+      <c r="C269">
+        <v>9719</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" s="1">
+        <v>44119</v>
+      </c>
+      <c r="B270">
+        <v>194362</v>
+      </c>
+      <c r="C270">
+        <v>9756</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" s="1">
+        <v>44120</v>
+      </c>
+      <c r="B271">
+        <v>196928</v>
+      </c>
+      <c r="C271">
+        <v>9781</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" s="1">
+        <v>44121</v>
+      </c>
+      <c r="B272">
+        <v>197067</v>
+      </c>
+      <c r="C272">
+        <v>9782</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" s="1">
+        <v>44122</v>
+      </c>
+      <c r="B273">
+        <v>200804</v>
+      </c>
+      <c r="C273">
+        <v>9816</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274" s="1">
+        <v>44123</v>
+      </c>
+      <c r="B274">
+        <v>204111</v>
+      </c>
+      <c r="C274">
+        <v>9832</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
+        <v>44124</v>
+      </c>
+      <c r="B275">
+        <v>206349</v>
+      </c>
+      <c r="C275">
+        <v>9849</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
+        <v>44125</v>
+      </c>
+      <c r="B276">
+        <v>209036</v>
+      </c>
+      <c r="C276">
+        <v>9883</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277" s="1">
+        <v>44126</v>
+      </c>
+      <c r="B277">
+        <v>211617</v>
+      </c>
+      <c r="C277">
+        <v>9916</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278" s="1">
+        <v>44127</v>
+      </c>
+      <c r="B278">
+        <v>214519</v>
+      </c>
+      <c r="C278">
+        <v>9940</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
+        <v>44128</v>
+      </c>
+      <c r="B279">
+        <v>216051</v>
+      </c>
+      <c r="C279">
+        <v>9969</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280" s="1">
+        <v>44129</v>
+      </c>
+      <c r="B280">
+        <v>218874</v>
+      </c>
+      <c r="C280">
+        <v>9995</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281" s="1">
+        <v>44130</v>
+      </c>
+      <c r="B281">
+        <v>222973</v>
+      </c>
+      <c r="C281">
+        <v>10026</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
+        <v>44131</v>
+      </c>
+      <c r="B282">
+        <v>225703</v>
+      </c>
+      <c r="C282">
+        <v>10052</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283" s="1">
+        <v>44132</v>
+      </c>
+      <c r="B283">
+        <v>228366</v>
+      </c>
+      <c r="C283">
+        <v>10084</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B284">
+        <v>231383</v>
+      </c>
+      <c r="C284">
+        <v>10127</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B285">
+        <v>234939</v>
+      </c>
+      <c r="C285">
+        <v>10163</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B286">
+        <v>237313</v>
+      </c>
+      <c r="C286">
+        <v>10187</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B287">
+        <v>239649</v>
+      </c>
+      <c r="C287">
+        <v>10230</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B288">
+        <v>243178</v>
+      </c>
+      <c r="C288">
+        <v>10262</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B289">
+        <v>247916</v>
+      </c>
+      <c r="C289">
+        <v>10334</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B290">
+        <v>250698</v>
+      </c>
+      <c r="C290">
+        <v>10385</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B291">
+        <v>253482</v>
+      </c>
+      <c r="C291">
+        <v>10432</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" s="1">
+        <v>44141</v>
+      </c>
+      <c r="B292">
+        <v>258875</v>
+      </c>
+      <c r="C292">
+        <v>10493</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" s="1">
+        <v>44142</v>
+      </c>
+      <c r="B293">
+        <v>263221</v>
+      </c>
+      <c r="C293">
+        <v>10547</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" s="1">
+        <v>44143</v>
+      </c>
+      <c r="B294">
+        <v>267165</v>
+      </c>
+      <c r="C294">
+        <v>10575</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" s="1">
+        <v>44144</v>
+      </c>
+      <c r="B295">
+        <v>272036</v>
+      </c>
+      <c r="C295">
+        <v>10620</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" s="1">
+        <v>44145</v>
+      </c>
+      <c r="B296">
+        <v>276481</v>
+      </c>
+      <c r="C296">
+        <v>10693</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" s="1">
+        <v>44146</v>
+      </c>
+      <c r="B297">
+        <v>280465</v>
+      </c>
+      <c r="C297">
+        <v>10748</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" s="1">
+        <v>44147</v>
+      </c>
+      <c r="B298">
+        <v>285939</v>
+      </c>
+      <c r="C298">
+        <v>10828</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" s="1">
+        <v>44148</v>
+      </c>
+      <c r="B299">
+        <v>290709</v>
+      </c>
+      <c r="C299">
+        <v>10885</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" s="1">
+        <v>44149</v>
+      </c>
+      <c r="B300">
+        <v>295139</v>
+      </c>
+      <c r="C300">
+        <v>10947</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" s="1">
+        <v>44150</v>
+      </c>
+      <c r="B301">
+        <v>299440</v>
+      </c>
+      <c r="C301">
+        <v>11001</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
+        <v>44151</v>
+      </c>
+      <c r="B302">
+        <v>305473</v>
+      </c>
+      <c r="C302">
+        <v>11075</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
+        <v>44152</v>
+      </c>
+      <c r="B303">
+        <v>309935</v>
+      </c>
+      <c r="C303">
+        <v>11136</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304" s="1">
+        <v>44153</v>
+      </c>
+      <c r="B304">
+        <v>314453</v>
+      </c>
+      <c r="C304">
+        <v>11238</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305" s="1">
+        <v>44154</v>
+      </c>
+      <c r="B305">
+        <v>319247</v>
+      </c>
+      <c r="C305">
+        <v>11314</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306" s="1">
+        <v>44155</v>
+      </c>
+      <c r="B306">
+        <v>324234</v>
+      </c>
+      <c r="C306">
+        <v>11385</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307" s="1">
+        <v>44156</v>
+      </c>
+      <c r="B307">
+        <v>329191</v>
+      </c>
+      <c r="C307">
+        <v>11455</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308" s="1">
+        <v>44157</v>
+      </c>
+      <c r="B308">
+        <v>333936</v>
+      </c>
+      <c r="C308">
+        <v>11502</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B309">
+        <v>340731</v>
+      </c>
+      <c r="C309">
+        <v>11570</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B310">
+        <v>346013</v>
+      </c>
+      <c r="C310">
+        <v>11676</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B311">
+        <v>350971</v>
+      </c>
+      <c r="C311">
+        <v>11733</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B312">
+        <v>356650</v>
+      </c>
+      <c r="C312">
+        <v>11818</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B313">
+        <v>362604</v>
+      </c>
+      <c r="C313">
+        <v>11916</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B314">
+        <v>368279</v>
+      </c>
+      <c r="C314">
+        <v>11993</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B315">
+        <v>373662</v>
+      </c>
+      <c r="C315">
+        <v>12046</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B316">
+        <v>381557</v>
+      </c>
+      <c r="C316">
+        <v>12147</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B317">
+        <v>387052</v>
+      </c>
+      <c r="C317">
+        <v>12229</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B318">
+        <v>393506</v>
+      </c>
+      <c r="C318">
+        <v>12342</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B319">
+        <v>399770</v>
+      </c>
+      <c r="C319">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320" s="1">
+        <v>44169</v>
+      </c>
+      <c r="B320">
+        <v>406189</v>
+      </c>
+      <c r="C320">
+        <v>12519</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A321" s="1">
+        <v>44170</v>
+      </c>
+      <c r="B321">
+        <v>412543</v>
+      </c>
+      <c r="C321">
+        <v>12607</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A322" s="1">
+        <v>44171</v>
+      </c>
+      <c r="B322">
+        <v>418848</v>
+      </c>
+      <c r="C322">
+        <v>12688</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A323" s="1">
+        <v>44172</v>
+      </c>
+      <c r="B323">
+        <v>426572</v>
+      </c>
+      <c r="C323">
+        <v>12796</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A324" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B324">
+        <v>432743</v>
+      </c>
+      <c r="C324">
+        <v>12887</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A325" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B325">
+        <v>439142</v>
+      </c>
+      <c r="C325">
+        <v>13009</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A326" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B326">
+        <v>445828</v>
+      </c>
+      <c r="C326">
+        <v>13130</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A327" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B327">
+        <v>452543</v>
+      </c>
+      <c r="C327">
+        <v>13267</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A328" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B328">
+        <v>458527</v>
+      </c>
+      <c r="C328">
+        <v>13367</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A329" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B329">
+        <v>464443</v>
+      </c>
+      <c r="C329">
+        <v>13451</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A330" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B330">
+        <v>472820</v>
+      </c>
+      <c r="C330">
+        <v>13570</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A331" s="1">
+        <v>44180</v>
+      </c>
+      <c r="B331">
+        <v>479064</v>
+      </c>
+      <c r="C331">
+        <v>13685</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A332" s="1">
+        <v>44181</v>
+      </c>
+      <c r="B332">
+        <v>485576</v>
+      </c>
+      <c r="C332">
+        <v>13815</v>
+      </c>
+    </row>
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1048576" s="1">
         <v>44045</v>
       </c>

</xml_diff>